<commit_message>
add coefficients confidence intervals
</commit_message>
<xml_diff>
--- a/CPUE/CPUE_MODELOS.xlsx
+++ b/CPUE/CPUE_MODELOS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macristina.perez\Documents\GitHub\BSB_PP\CPUE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5279B31-702A-49B2-B5DB-CE92FE77DF63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4AE5D4-B208-480A-8C0F-F54C5A34005A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Buzzards Bay" sheetId="6" r:id="rId1"/>
@@ -286,7 +286,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,6 +296,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -464,7 +470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -525,22 +531,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -555,9 +552,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -753,40 +760,40 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>0.84693591968449999</c:v>
+                  <c:v>2.332488957843172</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.114858229025</c:v>
+                  <c:v>3.0491358695737927</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.90957866569700008</c:v>
+                  <c:v>2.4832760235625106</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.5113800145000024E-2</c:v>
+                  <c:v>1.0997840035840882</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.9767068203890001</c:v>
+                  <c:v>7.2189305624475884</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.605592466409</c:v>
+                  <c:v>4.164407860422938</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4265740951449999</c:v>
+                  <c:v>3.8455739546061594</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.346922864797</c:v>
+                  <c:v>5.5180754003399874</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.7080291401345</c:v>
+                  <c:v>3.6928332460787581</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.306393980797</c:v>
+                  <c:v>3.9242587141337717</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.3671774707565001</c:v>
+                  <c:v>5.9003464158240995</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.7750110637344998</c:v>
+                  <c:v>1.3600655806948294</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1128,7 +1135,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:numFmt formatCode="0.00000" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1437,40 +1444,40 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>-1.2267990842355001</c:v>
+                  <c:v>0.29322968059422977</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.2192656545510001</c:v>
+                  <c:v>0.29544704747637934</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.3993862338750001</c:v>
+                  <c:v>0.24674836326173591</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-2.0369455549910001</c:v>
+                  <c:v>0.13042648360359665</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.7337604713564998</c:v>
+                  <c:v>2.0828985792779302</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-1.3959526894175001</c:v>
+                  <c:v>0.3186832567780461</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-1.1435575949350001</c:v>
+                  <c:v>1.0069832711184112</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.9590010049999625E-3</c:v>
+                  <c:v>0.60372824595138941</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.50463110621500018</c:v>
+                  <c:v>0.23017692615693536</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-1.468907021615</c:v>
+                  <c:v>0.43297772006315288</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.83706900712300014</c:v>
+                  <c:v>0.72206538999985292</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.32563957632350016</c:v>
+                  <c:v>0.29234897096634238</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1809,7 +1816,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:numFmt formatCode="0.00000" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2127,49 +2134,49 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-0.16197549120000002</c:v>
+                  <c:v>0.85046204808905101</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.24757856724999996</c:v>
+                  <c:v>1.2809199967920037</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.26696012125000002</c:v>
+                  <c:v>1.3059883641086991</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.2243288296</c:v>
+                  <c:v>1.2514824762571373</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.45269727359999995</c:v>
+                  <c:v>1.5725480626363486</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-6.7398649400000024E-2</c:v>
+                  <c:v>0.93482246063224628</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1774729692499999</c:v>
+                  <c:v>3.2461606814884179</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4580549586</c:v>
+                  <c:v>4.2975923986405551</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.4212398100500001</c:v>
+                  <c:v>4.1422528647095564</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0063159775999999</c:v>
+                  <c:v>2.7355047681947258</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.01790365525</c:v>
+                  <c:v>2.7673872810501194</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.98599635484999992</c:v>
+                  <c:v>2.6804812648837357</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.77690281285000007</c:v>
+                  <c:v>2.1747262897966491</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.96595025324999995</c:v>
+                  <c:v>2.6272830549181658</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.1447342600499999</c:v>
+                  <c:v>3.1416063955763178</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2541,7 +2548,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:numFmt formatCode="0.00000" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2859,49 +2866,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1.5418167457242424</c:v>
+                  <c:v>0.29566268665885315</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.241602777008973</c:v>
+                  <c:v>0.48285647661027475</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3578128358441579</c:v>
+                  <c:v>0.39935523930916778</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2419521233259834</c:v>
+                  <c:v>0.48258095313290528</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4897788504687313</c:v>
+                  <c:v>0.32189988816063853</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.7374714226395878</c:v>
+                  <c:v>0.21476656276109796</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.1311313940555462E-2</c:v>
+                  <c:v>3.4316559654626011</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.75187997813315333</c:v>
+                  <c:v>1.0747527705405528</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.3697207864885972</c:v>
+                  <c:v>0.39166062523904366</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0768723369496818</c:v>
+                  <c:v>0.63198261993735028</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.63340614439888687</c:v>
+                  <c:v>1.304288139132354</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.73263663861082196</c:v>
+                  <c:v>1.1090802904243526</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.1200775906282034</c:v>
+                  <c:v>0.58890896799593784</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.34444367726859165</c:v>
+                  <c:v>2.0912762585660429</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.31921677856983366</c:v>
+                  <c:v>2.1792725560688253</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7337,8 +7344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{368E9887-5155-46A1-B458-1CC08359F4C2}">
   <dimension ref="A1:O97"/>
   <sheetViews>
-    <sheetView topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="K79" sqref="K79:M92"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7347,7 +7354,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="29" t="s">
         <v>13</v>
       </c>
     </row>
@@ -7386,13 +7393,13 @@
       </c>
       <c r="J6" s="24"/>
       <c r="K6" s="25"/>
-      <c r="L6" s="26" t="s">
+      <c r="L6" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="M6" s="27" t="s">
+      <c r="M6" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="N6" s="33" t="s">
+      <c r="N6" s="30" t="s">
         <v>64</v>
       </c>
     </row>
@@ -7426,18 +7433,18 @@
         <f t="shared" ref="I7:I18" si="1">H7/2</f>
         <v>4.7391968449999998E-4</v>
       </c>
-      <c r="K7" s="28">
+      <c r="K7" s="27">
         <v>2008</v>
       </c>
-      <c r="L7" s="29">
-        <f>(B7+I7)</f>
-        <v>0.84693591968449999</v>
-      </c>
-      <c r="M7" s="36">
+      <c r="L7" s="36">
+        <f>EXP(B7+I7)</f>
+        <v>2.332488957843172</v>
+      </c>
+      <c r="M7" s="33">
         <f>L7/AVERAGE($L$7:$L$19)</f>
-        <v>0.6565863618516049</v>
-      </c>
-      <c r="N7" s="34">
+        <v>0.62772783969625845</v>
+      </c>
+      <c r="N7" s="31">
         <v>2.58</v>
       </c>
       <c r="O7">
@@ -7475,18 +7482,18 @@
         <f t="shared" si="1"/>
         <v>6.9530934049999991E-4</v>
       </c>
-      <c r="K8" s="28">
+      <c r="K8" s="27">
         <v>2009</v>
       </c>
-      <c r="L8" s="29">
-        <f>($B$7+$I$7+B8+I8)</f>
-        <v>1.114858229025</v>
-      </c>
-      <c r="M8" s="36">
+      <c r="L8" s="36">
+        <f>EXP($B$7+$I$7+B8+I8)</f>
+        <v>3.0491358695737927</v>
+      </c>
+      <c r="M8" s="33">
         <f>L8/AVERAGE($L$7:$L$19)</f>
-        <v>0.86429290760100541</v>
-      </c>
-      <c r="N8" s="34">
+        <v>0.82059444093480738</v>
+      </c>
+      <c r="N8" s="31">
         <v>2.87</v>
       </c>
     </row>
@@ -7517,18 +7524,18 @@
         <f t="shared" si="1"/>
         <v>7.5874601249999987E-4</v>
       </c>
-      <c r="K9" s="28">
+      <c r="K9" s="27">
         <v>2010</v>
       </c>
-      <c r="L9" s="29">
-        <f t="shared" ref="L9:L11" si="2">($B$7+$I$7+B9+I9)</f>
-        <v>0.90957866569700008</v>
-      </c>
-      <c r="M9" s="36">
+      <c r="L9" s="36">
+        <f t="shared" ref="L9:L19" si="2">EXP($B$7+$I$7+B9+I9)</f>
+        <v>2.4832760235625106</v>
+      </c>
+      <c r="M9" s="33">
         <f>L9/AVERAGE($L$7:$L$19)</f>
-        <v>0.70515009819196872</v>
-      </c>
-      <c r="N9" s="34">
+        <v>0.66830819858707302</v>
+      </c>
+      <c r="N9" s="31">
         <v>2.35</v>
       </c>
     </row>
@@ -7562,18 +7569,18 @@
         <f t="shared" si="1"/>
         <v>1.6438804605E-3</v>
       </c>
-      <c r="K10" s="28">
+      <c r="K10" s="27">
         <v>2011</v>
       </c>
-      <c r="L10" s="29">
+      <c r="L10" s="36">
         <f t="shared" si="2"/>
-        <v>9.5113800145000024E-2</v>
-      </c>
-      <c r="M10" s="36">
+        <v>1.0997840035840882</v>
+      </c>
+      <c r="M10" s="33">
         <f>L10/AVERAGE($L$7:$L$19)</f>
-        <v>7.3736893840032444E-2</v>
-      </c>
-      <c r="N10" s="34">
+        <v>0.29597783705725023</v>
+      </c>
+      <c r="N10" s="31">
         <v>1.1200000000000001</v>
       </c>
     </row>
@@ -7607,18 +7614,18 @@
         <f t="shared" si="1"/>
         <v>5.0890070450000007E-4</v>
       </c>
-      <c r="K11" s="28">
+      <c r="K11" s="27">
         <v>2012</v>
       </c>
-      <c r="L11" s="29">
+      <c r="L11" s="36">
         <f t="shared" si="2"/>
-        <v>1.9767068203890001</v>
-      </c>
-      <c r="M11" s="36">
+        <v>7.2189305624475884</v>
+      </c>
+      <c r="M11" s="33">
         <f>L11/AVERAGE($L$7:$L$19)</f>
-        <v>1.5324403056726563</v>
-      </c>
-      <c r="N11" s="34">
+        <v>1.9427846256870482</v>
+      </c>
+      <c r="N11" s="31">
         <v>8.49</v>
       </c>
     </row>
@@ -7652,12 +7659,12 @@
         <f t="shared" si="1"/>
         <v>6.8054672450000011E-4</v>
       </c>
-      <c r="K12" s="28">
+      <c r="K12" s="27">
         <v>2013</v>
       </c>
-      <c r="L12" s="29"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="34"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="31"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -7689,18 +7696,18 @@
         <f t="shared" si="1"/>
         <v>7.0917546050000004E-4</v>
       </c>
-      <c r="K13" s="28">
+      <c r="K13" s="27">
         <v>2014</v>
       </c>
-      <c r="L13" s="29">
-        <f>($B$7+$I$7+B12+I12)</f>
-        <v>1.605592466409</v>
-      </c>
-      <c r="M13" s="36">
+      <c r="L13" s="36">
+        <f t="shared" si="2"/>
+        <v>4.164407860422938</v>
+      </c>
+      <c r="M13" s="33">
         <f t="shared" ref="M13:M19" si="3">L13/AVERAGE($L$7:$L$19)</f>
-        <v>1.244734213809876</v>
-      </c>
-      <c r="N13" s="34">
+        <v>1.1207404609772098</v>
+      </c>
+      <c r="N13" s="31">
         <v>5.14</v>
       </c>
     </row>
@@ -7734,18 +7741,18 @@
         <f t="shared" si="1"/>
         <v>6.8394511249999991E-4</v>
       </c>
-      <c r="K14" s="28">
+      <c r="K14" s="27">
         <v>2015</v>
       </c>
-      <c r="L14" s="29">
-        <f t="shared" ref="L14:L19" si="4">($B$7+$I$7+B13+I13)</f>
-        <v>1.4265740951449999</v>
-      </c>
-      <c r="M14" s="36">
+      <c r="L14" s="36">
+        <f t="shared" si="2"/>
+        <v>3.8455739546061594</v>
+      </c>
+      <c r="M14" s="33">
         <f t="shared" si="3"/>
-        <v>1.1059503715368786</v>
-      </c>
-      <c r="N14" s="34">
+        <v>1.0349347304731928</v>
+      </c>
+      <c r="N14" s="31">
         <v>4.12</v>
       </c>
     </row>
@@ -7779,18 +7786,18 @@
         <f t="shared" si="1"/>
         <v>6.6722044999999999E-4</v>
       </c>
-      <c r="K15" s="28">
+      <c r="K15" s="27">
         <v>2016</v>
       </c>
-      <c r="L15" s="29">
-        <f t="shared" si="4"/>
-        <v>1.346922864797</v>
-      </c>
-      <c r="M15" s="36">
+      <c r="L15" s="36">
+        <f t="shared" si="2"/>
+        <v>5.5180754003399874</v>
+      </c>
+      <c r="M15" s="33">
         <f t="shared" si="3"/>
-        <v>1.044200821971571</v>
-      </c>
-      <c r="N15" s="34">
+        <v>1.4850443508806455</v>
+      </c>
+      <c r="N15" s="31">
         <v>3.79</v>
       </c>
     </row>
@@ -7824,18 +7831,18 @@
         <f t="shared" si="1"/>
         <v>5.9806111249999987E-4</v>
       </c>
-      <c r="K16" s="28">
+      <c r="K16" s="27">
         <v>2017</v>
       </c>
-      <c r="L16" s="29">
-        <f t="shared" si="4"/>
-        <v>1.7080291401345</v>
-      </c>
-      <c r="M16" s="36">
+      <c r="L16" s="36">
+        <f t="shared" si="2"/>
+        <v>3.6928332460787581</v>
+      </c>
+      <c r="M16" s="33">
         <f t="shared" si="3"/>
-        <v>1.3241481592553133</v>
-      </c>
-      <c r="N16" s="34">
+        <v>0.9938286001846961</v>
+      </c>
+      <c r="N16" s="31">
         <v>5.43</v>
       </c>
     </row>
@@ -7869,18 +7876,18 @@
         <f t="shared" si="1"/>
         <v>6.3055107200000007E-4</v>
       </c>
-      <c r="K17" s="28">
+      <c r="K17" s="27">
         <v>2018</v>
       </c>
-      <c r="L17" s="29">
-        <f t="shared" si="4"/>
-        <v>1.306393980797</v>
-      </c>
-      <c r="M17" s="36">
+      <c r="L17" s="36">
+        <f t="shared" si="2"/>
+        <v>3.9242587141337717</v>
+      </c>
+      <c r="M17" s="33">
         <f t="shared" si="3"/>
-        <v>1.0127808386210257</v>
-      </c>
-      <c r="N17" s="34">
+        <v>1.0561106567082137</v>
+      </c>
+      <c r="N17" s="31">
         <v>3.84</v>
       </c>
     </row>
@@ -7914,18 +7921,18 @@
         <f t="shared" si="1"/>
         <v>5.6414405000000006E-4</v>
       </c>
-      <c r="K18" s="28">
+      <c r="K18" s="27">
         <v>2019</v>
       </c>
-      <c r="L18" s="29">
-        <f t="shared" si="4"/>
-        <v>1.3671774707565001</v>
-      </c>
-      <c r="M18" s="36">
+      <c r="L18" s="36">
+        <f t="shared" si="2"/>
+        <v>5.9003464158240995</v>
+      </c>
+      <c r="M18" s="33">
         <f t="shared" si="3"/>
-        <v>1.0599031882646905</v>
-      </c>
-      <c r="N18" s="34">
+        <v>1.5879225051036034</v>
+      </c>
+      <c r="N18" s="31">
         <v>3.77</v>
       </c>
     </row>
@@ -7948,18 +7955,18 @@
       <c r="F19" t="s">
         <v>21</v>
       </c>
-      <c r="K19" s="30">
+      <c r="K19" s="28">
         <v>2020</v>
       </c>
-      <c r="L19" s="31">
-        <f t="shared" si="4"/>
-        <v>1.7750110637344998</v>
-      </c>
-      <c r="M19" s="37">
+      <c r="L19" s="37">
+        <f t="shared" si="2"/>
+        <v>1.3600655806948294</v>
+      </c>
+      <c r="M19" s="34">
         <f t="shared" si="3"/>
-        <v>1.376075839383379</v>
-      </c>
-      <c r="N19" s="35">
+        <v>0.36602575371000129</v>
+      </c>
+      <c r="N19" s="32">
         <v>5.64</v>
       </c>
     </row>
@@ -8046,7 +8053,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="29" t="s">
         <v>14</v>
       </c>
       <c r="F28" s="14"/>
@@ -8080,13 +8087,13 @@
       </c>
       <c r="J31" s="24"/>
       <c r="K31" s="25"/>
-      <c r="L31" s="26" t="s">
+      <c r="L31" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="M31" s="27" t="s">
+      <c r="M31" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="N31" s="33" t="s">
+      <c r="N31" s="30" t="s">
         <v>64</v>
       </c>
     </row>
@@ -8113,25 +8120,25 @@
         <v>2008</v>
       </c>
       <c r="H32">
-        <f t="shared" ref="H32:H43" si="5">C32^2</f>
+        <f t="shared" ref="H32:H43" si="4">C32^2</f>
         <v>4.9318315289999994E-3</v>
       </c>
       <c r="I32">
-        <f t="shared" ref="I32:I43" si="6">H32/2</f>
+        <f t="shared" ref="I32:I43" si="5">H32/2</f>
         <v>2.4659157644999997E-3</v>
       </c>
-      <c r="K32" s="28">
+      <c r="K32" s="27">
         <v>2008</v>
       </c>
-      <c r="L32" s="29">
-        <f>(B32+I32)</f>
-        <v>-1.2267990842355001</v>
-      </c>
-      <c r="M32" s="36">
+      <c r="L32" s="36">
+        <f>EXP(B32+I32)</f>
+        <v>0.29322968059422977</v>
+      </c>
+      <c r="M32" s="33">
         <f>L32/AVERAGE($L$32:$L$44)</f>
-        <v>1.3609132204114487</v>
-      </c>
-      <c r="N32" s="34">
+        <v>0.52868200186546066</v>
+      </c>
+      <c r="N32" s="31">
         <v>0.53500000000000003</v>
       </c>
     </row>
@@ -8155,25 +8162,25 @@
         <v>2009</v>
       </c>
       <c r="H33">
+        <f t="shared" si="4"/>
+        <v>6.8828593689999988E-3</v>
+      </c>
+      <c r="I33">
         <f t="shared" si="5"/>
-        <v>6.8828593689999988E-3</v>
-      </c>
-      <c r="I33">
-        <f t="shared" si="6"/>
         <v>3.4414296844999994E-3</v>
       </c>
-      <c r="K33" s="28">
+      <c r="K33" s="27">
         <v>2009</v>
       </c>
-      <c r="L33" s="29">
-        <f>($B$32+$I$32+B33+I33)</f>
-        <v>-1.2192656545510001</v>
-      </c>
-      <c r="M33" s="36">
+      <c r="L33" s="36">
+        <f>EXP($B$32+$I$32+B33+I33)</f>
+        <v>0.29544704747637934</v>
+      </c>
+      <c r="M33" s="33">
         <f>L33/AVERAGE($L$32:$L$44)</f>
-        <v>1.3525562333673435</v>
-      </c>
-      <c r="N33" s="34">
+        <v>0.53267983032453547</v>
+      </c>
+      <c r="N33" s="31">
         <v>0.52700000000000002</v>
       </c>
     </row>
@@ -8200,25 +8207,25 @@
         <v>2010</v>
       </c>
       <c r="H34">
+        <f t="shared" si="4"/>
+        <v>7.4717007210000005E-3</v>
+      </c>
+      <c r="I34">
         <f t="shared" si="5"/>
-        <v>7.4717007210000005E-3</v>
-      </c>
-      <c r="I34">
-        <f t="shared" si="6"/>
         <v>3.7358503605000003E-3</v>
       </c>
-      <c r="K34" s="28">
+      <c r="K34" s="27">
         <v>2010</v>
       </c>
-      <c r="L34" s="29">
-        <f t="shared" ref="L34:L36" si="7">($B$32+$I$32+B34+I34)</f>
-        <v>-1.3993862338750001</v>
-      </c>
-      <c r="M34" s="36">
+      <c r="L34" s="36">
+        <f t="shared" ref="L34:L44" si="6">EXP($B$32+$I$32+B34+I34)</f>
+        <v>0.24674836326173591</v>
+      </c>
+      <c r="M34" s="33">
         <f>L34/AVERAGE($L$32:$L$44)</f>
-        <v>1.552367662003155</v>
-      </c>
-      <c r="N34" s="34">
+        <v>0.44487794817318871</v>
+      </c>
+      <c r="N34" s="31">
         <v>0.44500000000000001</v>
       </c>
     </row>
@@ -8245,25 +8252,25 @@
         <v>2011</v>
       </c>
       <c r="H35">
+        <f t="shared" si="4"/>
+        <v>1.4145058488999999E-2</v>
+      </c>
+      <c r="I35">
         <f t="shared" si="5"/>
-        <v>1.4145058488999999E-2</v>
-      </c>
-      <c r="I35">
+        <v>7.0725292444999994E-3</v>
+      </c>
+      <c r="K35" s="27">
+        <v>2011</v>
+      </c>
+      <c r="L35" s="36">
         <f t="shared" si="6"/>
-        <v>7.0725292444999994E-3</v>
-      </c>
-      <c r="K35" s="28">
-        <v>2011</v>
-      </c>
-      <c r="L35" s="29">
-        <f t="shared" si="7"/>
-        <v>-2.0369455549910001</v>
-      </c>
-      <c r="M35" s="36">
+        <v>0.13042648360359665</v>
+      </c>
+      <c r="M35" s="33">
         <f>L35/AVERAGE($L$32:$L$44)</f>
-        <v>2.2596252073118155</v>
-      </c>
-      <c r="N35" s="34">
+        <v>0.23515400728905292</v>
+      </c>
+      <c r="N35" s="31">
         <v>0.26700000000000002</v>
       </c>
     </row>
@@ -8290,25 +8297,25 @@
         <v>2012</v>
       </c>
       <c r="H36">
+        <f t="shared" si="4"/>
+        <v>4.0231111839999995E-3</v>
+      </c>
+      <c r="I36">
         <f t="shared" si="5"/>
-        <v>4.0231111839999995E-3</v>
-      </c>
-      <c r="I36">
+        <v>2.0115555919999997E-3</v>
+      </c>
+      <c r="K36" s="27">
+        <v>2012</v>
+      </c>
+      <c r="L36" s="36">
         <f t="shared" si="6"/>
-        <v>2.0115555919999997E-3</v>
-      </c>
-      <c r="K36" s="28">
-        <v>2012</v>
-      </c>
-      <c r="L36" s="29">
-        <f t="shared" si="7"/>
-        <v>0.7337604713564998</v>
-      </c>
-      <c r="M36" s="36">
+        <v>2.0828985792779302</v>
+      </c>
+      <c r="M36" s="33">
         <f>L36/AVERAGE($L$32:$L$44)</f>
-        <v>-0.81397544138752009</v>
-      </c>
-      <c r="N36" s="34">
+        <v>3.7553872048143875</v>
+      </c>
+      <c r="N36" s="31">
         <v>4.12</v>
       </c>
     </row>
@@ -8335,18 +8342,19 @@
         <v>2014</v>
       </c>
       <c r="H37">
+        <f t="shared" si="4"/>
+        <v>9.1787896360000006E-3</v>
+      </c>
+      <c r="I37">
         <f t="shared" si="5"/>
-        <v>9.1787896360000006E-3</v>
-      </c>
-      <c r="I37">
-        <f t="shared" si="6"/>
         <v>4.5893948180000003E-3</v>
       </c>
-      <c r="K37" s="28">
+      <c r="K37" s="27">
         <v>2013</v>
       </c>
-      <c r="M37" s="36"/>
-      <c r="N37" s="34"/>
+      <c r="L37" s="36"/>
+      <c r="M37" s="33"/>
+      <c r="N37" s="31"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
@@ -8368,25 +8376,25 @@
         <v>2015</v>
       </c>
       <c r="H38">
+        <f t="shared" si="4"/>
+        <v>7.7529786010000004E-3</v>
+      </c>
+      <c r="I38">
         <f t="shared" si="5"/>
-        <v>7.7529786010000004E-3</v>
-      </c>
-      <c r="I38">
+        <v>3.8764893005000002E-3</v>
+      </c>
+      <c r="K38" s="27">
+        <v>2014</v>
+      </c>
+      <c r="L38" s="36">
         <f t="shared" si="6"/>
-        <v>3.8764893005000002E-3</v>
-      </c>
-      <c r="K38" s="28">
-        <v>2014</v>
-      </c>
-      <c r="L38" s="29">
-        <f>($B$32+$I$32+B37+I37)</f>
-        <v>-1.3959526894175001</v>
-      </c>
-      <c r="M38" s="36">
-        <f t="shared" ref="M38:M44" si="8">L38/AVERAGE($L$32:$L$44)</f>
-        <v>1.5485587611773168</v>
-      </c>
-      <c r="N38" s="34">
+        <v>0.3186832567780461</v>
+      </c>
+      <c r="M38" s="33">
+        <f t="shared" ref="M38:M44" si="7">L38/AVERAGE($L$32:$L$44)</f>
+        <v>0.57457383513494675</v>
+      </c>
+      <c r="N38" s="31">
         <v>0.51700000000000002</v>
       </c>
     </row>
@@ -8413,25 +8421,25 @@
         <v>2016</v>
       </c>
       <c r="H39">
+        <f t="shared" si="4"/>
+        <v>4.6841704809999999E-3</v>
+      </c>
+      <c r="I39">
         <f t="shared" si="5"/>
-        <v>4.6841704809999999E-3</v>
-      </c>
-      <c r="I39">
+        <v>2.3420852404999999E-3</v>
+      </c>
+      <c r="K39" s="27">
+        <v>2015</v>
+      </c>
+      <c r="L39" s="36">
         <f t="shared" si="6"/>
-        <v>2.3420852404999999E-3</v>
-      </c>
-      <c r="K39" s="28">
-        <v>2015</v>
-      </c>
-      <c r="L39" s="29">
-        <f t="shared" ref="L39:L44" si="9">($B$32+$I$32+B38+I38)</f>
-        <v>-1.1435575949350001</v>
-      </c>
-      <c r="M39" s="36">
-        <f t="shared" si="8"/>
-        <v>1.2685717402689332</v>
-      </c>
-      <c r="N39" s="34">
+        <v>1.0069832711184112</v>
+      </c>
+      <c r="M39" s="33">
+        <f t="shared" si="7"/>
+        <v>1.8155526771405137</v>
+      </c>
+      <c r="N39" s="31">
         <v>0.625</v>
       </c>
     </row>
@@ -8458,25 +8466,25 @@
         <v>2017</v>
       </c>
       <c r="H40">
+        <f t="shared" si="4"/>
+        <v>6.1119560409999994E-3</v>
+      </c>
+      <c r="I40">
         <f t="shared" si="5"/>
-        <v>6.1119560409999994E-3</v>
-      </c>
-      <c r="I40">
+        <v>3.0559780204999997E-3</v>
+      </c>
+      <c r="K40" s="27">
+        <v>2016</v>
+      </c>
+      <c r="L40" s="36">
         <f t="shared" si="6"/>
-        <v>3.0559780204999997E-3</v>
-      </c>
-      <c r="K40" s="28">
-        <v>2016</v>
-      </c>
-      <c r="L40" s="29">
-        <f t="shared" si="9"/>
-        <v>6.9590010049999625E-3</v>
-      </c>
-      <c r="M40" s="36">
-        <f t="shared" si="8"/>
-        <v>-7.7197616058400989E-3</v>
-      </c>
-      <c r="N40" s="34">
+        <v>0.60372824595138941</v>
+      </c>
+      <c r="M40" s="33">
+        <f t="shared" si="7"/>
+        <v>1.0884991485360049</v>
+      </c>
+      <c r="N40" s="31">
         <v>1.96</v>
       </c>
     </row>
@@ -8503,25 +8511,25 @@
         <v>2018</v>
       </c>
       <c r="H41">
+        <f t="shared" si="4"/>
+        <v>7.7741252410000001E-3</v>
+      </c>
+      <c r="I41">
         <f t="shared" si="5"/>
-        <v>7.7741252410000001E-3</v>
-      </c>
-      <c r="I41">
+        <v>3.8870626205000001E-3</v>
+      </c>
+      <c r="K41" s="27">
+        <v>2017</v>
+      </c>
+      <c r="L41" s="36">
         <f t="shared" si="6"/>
-        <v>3.8870626205000001E-3</v>
-      </c>
-      <c r="K41" s="28">
-        <v>2017</v>
-      </c>
-      <c r="L41" s="29">
-        <f t="shared" si="9"/>
-        <v>-0.50463110621500018</v>
-      </c>
-      <c r="M41" s="36">
-        <f t="shared" si="8"/>
-        <v>0.55979756808085079</v>
-      </c>
-      <c r="N41" s="34">
+        <v>0.23017692615693536</v>
+      </c>
+      <c r="M41" s="33">
+        <f t="shared" si="7"/>
+        <v>0.41500027506520276</v>
+      </c>
+      <c r="N41" s="31">
         <v>1.1599999999999999</v>
       </c>
     </row>
@@ -8548,25 +8556,25 @@
         <v>2019</v>
       </c>
       <c r="H42">
+        <f t="shared" si="4"/>
+        <v>5.8041542250000001E-3</v>
+      </c>
+      <c r="I42">
         <f t="shared" si="5"/>
-        <v>5.8041542250000001E-3</v>
-      </c>
-      <c r="I42">
+        <v>2.9020771125000001E-3</v>
+      </c>
+      <c r="K42" s="27">
+        <v>2018</v>
+      </c>
+      <c r="L42" s="36">
         <f t="shared" si="6"/>
-        <v>2.9020771125000001E-3</v>
-      </c>
-      <c r="K42" s="28">
-        <v>2018</v>
-      </c>
-      <c r="L42" s="29">
-        <f t="shared" si="9"/>
-        <v>-1.468907021615</v>
-      </c>
-      <c r="M42" s="36">
-        <f t="shared" si="8"/>
-        <v>1.6294884883426555</v>
-      </c>
-      <c r="N42" s="34">
+        <v>0.43297772006315288</v>
+      </c>
+      <c r="M42" s="33">
+        <f t="shared" si="7"/>
+        <v>0.78064242112957238</v>
+      </c>
+      <c r="N42" s="31">
         <v>0.41699999999999998</v>
       </c>
     </row>
@@ -8593,25 +8601,25 @@
         <v>2020</v>
       </c>
       <c r="H43">
+        <f t="shared" si="4"/>
+        <v>5.0030158240000006E-3</v>
+      </c>
+      <c r="I43">
         <f t="shared" si="5"/>
-        <v>5.0030158240000006E-3</v>
-      </c>
-      <c r="I43">
+        <v>2.5015079120000003E-3</v>
+      </c>
+      <c r="K43" s="27">
+        <v>2019</v>
+      </c>
+      <c r="L43" s="36">
         <f t="shared" si="6"/>
-        <v>2.5015079120000003E-3</v>
-      </c>
-      <c r="K43" s="28">
-        <v>2019</v>
-      </c>
-      <c r="L43" s="29">
-        <f t="shared" si="9"/>
-        <v>-0.83706900712300014</v>
-      </c>
-      <c r="M43" s="36">
-        <f t="shared" si="8"/>
-        <v>0.92857770504472914</v>
-      </c>
-      <c r="N43" s="34">
+        <v>0.72206538999985292</v>
+      </c>
+      <c r="M43" s="33">
+        <f t="shared" si="7"/>
+        <v>1.3018565347453401</v>
+      </c>
+      <c r="N43" s="31">
         <v>0.79300000000000004</v>
       </c>
     </row>
@@ -8631,18 +8639,18 @@
       <c r="E44" s="14">
         <v>0.95652999999999999</v>
       </c>
-      <c r="K44" s="30">
+      <c r="K44" s="28">
         <v>2020</v>
       </c>
-      <c r="L44" s="31">
-        <f t="shared" si="9"/>
-        <v>-0.32563957632350016</v>
-      </c>
-      <c r="M44" s="37">
-        <f t="shared" si="8"/>
-        <v>0.36123861698511228</v>
-      </c>
-      <c r="N44" s="35">
+      <c r="L44" s="37">
+        <f t="shared" si="6"/>
+        <v>0.29234897096634238</v>
+      </c>
+      <c r="M44" s="34">
+        <f t="shared" si="7"/>
+        <v>0.52709411578179377</v>
+      </c>
+      <c r="N44" s="32">
         <v>1.36</v>
       </c>
     </row>
@@ -8732,7 +8740,7 @@
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A51" s="32" t="s">
+      <c r="A51" s="29" t="s">
         <v>19</v>
       </c>
       <c r="E51" s="14"/>
@@ -8766,10 +8774,10 @@
       </c>
       <c r="J55" s="24"/>
       <c r="K55" s="25"/>
-      <c r="L55" s="26" t="s">
+      <c r="L55" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="M55" s="27" t="s">
+      <c r="M55" s="26" t="s">
         <v>38</v>
       </c>
       <c r="N55" s="24"/>
@@ -8801,17 +8809,17 @@
         <v>3.6072036000000004E-3</v>
       </c>
       <c r="I56">
-        <f t="shared" ref="I56:I67" si="10">H56/2</f>
+        <f t="shared" ref="I56:I67" si="8">H56/2</f>
         <v>1.8036018000000002E-3</v>
       </c>
-      <c r="K56" s="28">
+      <c r="K56" s="27">
         <v>2008</v>
       </c>
-      <c r="L56" s="29">
+      <c r="L56" s="38">
         <f>EXP(B56+I56)</f>
         <v>2.2498726211690334</v>
       </c>
-      <c r="M56" s="36">
+      <c r="M56" s="33">
         <f>L56/AVERAGE($L$56:$L$68)</f>
         <v>0.53824065273791077</v>
       </c>
@@ -8839,21 +8847,21 @@
         <v>2009</v>
       </c>
       <c r="H57">
-        <f t="shared" ref="H57:H66" si="11">C57^2</f>
+        <f t="shared" ref="H57:H66" si="9">C57^2</f>
         <v>5.1696100000000007E-3</v>
       </c>
       <c r="I57">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>2.5848050000000003E-3</v>
       </c>
-      <c r="K57" s="28">
+      <c r="K57" s="27">
         <v>2009</v>
       </c>
-      <c r="L57" s="29">
+      <c r="L57" s="38">
         <f>EXP($B$56+$I$56+B57+I57)</f>
         <v>3.1748754613382846</v>
       </c>
-      <c r="M57" s="36">
+      <c r="M57" s="33">
         <f>L57/AVERAGE($L$56:$L$68)</f>
         <v>0.75953057279499558</v>
       </c>
@@ -8881,21 +8889,21 @@
         <v>2010</v>
       </c>
       <c r="H58">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>5.2316289000000011E-3</v>
       </c>
       <c r="I58">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>2.6158144500000005E-3</v>
       </c>
-      <c r="K58" s="28">
+      <c r="K58" s="27">
         <v>2010</v>
       </c>
-      <c r="L58" s="29">
-        <f t="shared" ref="L58:L60" si="12">EXP($B$56+$I$56+B58+I58)</f>
+      <c r="L58" s="38">
+        <f t="shared" ref="L58:L60" si="10">EXP($B$56+$I$56+B58+I58)</f>
         <v>2.7505184364339637</v>
       </c>
-      <c r="M58" s="36">
+      <c r="M58" s="33">
         <f>L58/AVERAGE($L$56:$L$68)</f>
         <v>0.65801095789353514</v>
       </c>
@@ -8923,21 +8931,21 @@
         <v>2011</v>
       </c>
       <c r="H59">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>8.0928015999999995E-3</v>
       </c>
       <c r="I59">
+        <f t="shared" si="8"/>
+        <v>4.0464007999999997E-3</v>
+      </c>
+      <c r="K59" s="27">
+        <v>2011</v>
+      </c>
+      <c r="L59" s="38">
         <f t="shared" si="10"/>
-        <v>4.0464007999999997E-3</v>
-      </c>
-      <c r="K59" s="28">
-        <v>2011</v>
-      </c>
-      <c r="L59" s="29">
-        <f t="shared" si="12"/>
         <v>1.1737573372042136</v>
       </c>
-      <c r="M59" s="36">
+      <c r="M59" s="33">
         <f>L59/AVERAGE($L$56:$L$68)</f>
         <v>0.28079985924022827</v>
       </c>
@@ -8965,21 +8973,21 @@
         <v>2012</v>
       </c>
       <c r="H60">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>5.3890281000000002E-3</v>
       </c>
       <c r="I60">
+        <f t="shared" si="8"/>
+        <v>2.6945140500000001E-3</v>
+      </c>
+      <c r="K60" s="27">
+        <v>2012</v>
+      </c>
+      <c r="L60" s="38">
         <f t="shared" si="10"/>
-        <v>2.6945140500000001E-3</v>
-      </c>
-      <c r="K60" s="28">
-        <v>2012</v>
-      </c>
-      <c r="L60" s="29">
-        <f t="shared" si="12"/>
         <v>6.7374270980496984</v>
       </c>
-      <c r="M60" s="36">
+      <c r="M60" s="33">
         <f>L60/AVERAGE($L$56:$L$68)</f>
         <v>1.6118055417484494</v>
       </c>
@@ -9007,17 +9015,18 @@
         <v>2014</v>
       </c>
       <c r="H61">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>6.241E-3</v>
       </c>
       <c r="I61">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>3.1205E-3</v>
       </c>
-      <c r="K61" s="28">
+      <c r="K61" s="27">
         <v>2013</v>
       </c>
-      <c r="M61" s="36"/>
+      <c r="L61" s="39"/>
+      <c r="M61" s="33"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
@@ -9042,22 +9051,22 @@
         <v>2015</v>
       </c>
       <c r="H62">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>5.9459520999999996E-3</v>
       </c>
       <c r="I62">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>2.9729760499999998E-3</v>
       </c>
-      <c r="K62" s="28">
+      <c r="K62" s="27">
         <v>2014</v>
       </c>
-      <c r="L62" s="29">
-        <f t="shared" ref="L62:L68" si="13">EXP($B$56+$I$56+B61+I61)</f>
+      <c r="L62" s="38">
+        <f t="shared" ref="L62:L68" si="11">EXP($B$56+$I$56+B61+I61)</f>
         <v>5.0202217287403705</v>
       </c>
-      <c r="M62" s="36">
-        <f t="shared" ref="M62:M68" si="14">L62/AVERAGE($L$56:$L$68)</f>
+      <c r="M62" s="33">
+        <f t="shared" ref="M62:M68" si="12">L62/AVERAGE($L$56:$L$68)</f>
         <v>1.200995734043937</v>
       </c>
     </row>
@@ -9084,22 +9093,22 @@
         <v>2016</v>
       </c>
       <c r="H63">
+        <f t="shared" si="9"/>
+        <v>5.5935440999999994E-3</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="8"/>
+        <v>2.7967720499999997E-3</v>
+      </c>
+      <c r="K63" s="27">
+        <v>2015</v>
+      </c>
+      <c r="L63" s="38">
         <f t="shared" si="11"/>
-        <v>5.5935440999999994E-3</v>
-      </c>
-      <c r="I63">
-        <f t="shared" si="10"/>
-        <v>2.7967720499999997E-3</v>
-      </c>
-      <c r="K63" s="28">
-        <v>2015</v>
-      </c>
-      <c r="L63" s="29">
-        <f t="shared" si="13"/>
         <v>4.717111197735985</v>
       </c>
-      <c r="M63" s="36">
-        <f t="shared" si="14"/>
+      <c r="M63" s="33">
+        <f t="shared" si="12"/>
         <v>1.1284821132618128</v>
       </c>
     </row>
@@ -9126,22 +9135,22 @@
         <v>2017</v>
       </c>
       <c r="H64">
+        <f t="shared" si="9"/>
+        <v>6.2552280999999986E-3</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="8"/>
+        <v>3.1276140499999993E-3</v>
+      </c>
+      <c r="K64" s="27">
+        <v>2016</v>
+      </c>
+      <c r="L64" s="38">
         <f t="shared" si="11"/>
-        <v>6.2552280999999986E-3</v>
-      </c>
-      <c r="I64">
-        <f t="shared" si="10"/>
-        <v>3.1276140499999993E-3</v>
-      </c>
-      <c r="K64" s="28">
-        <v>2016</v>
-      </c>
-      <c r="L64" s="29">
-        <f t="shared" si="13"/>
         <v>3.8823489651823988</v>
       </c>
-      <c r="M64" s="36">
-        <f t="shared" si="14"/>
+      <c r="M64" s="33">
+        <f t="shared" si="12"/>
         <v>0.92878059918358902</v>
       </c>
     </row>
@@ -9168,22 +9177,22 @@
         <v>2018</v>
       </c>
       <c r="H65">
+        <f t="shared" si="9"/>
+        <v>4.9126081000000002E-3</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="8"/>
+        <v>2.4563040500000001E-3</v>
+      </c>
+      <c r="K65" s="27">
+        <v>2017</v>
+      </c>
+      <c r="L65" s="38">
         <f t="shared" si="11"/>
-        <v>4.9126081000000002E-3</v>
-      </c>
-      <c r="I65">
-        <f t="shared" si="10"/>
-        <v>2.4563040500000001E-3</v>
-      </c>
-      <c r="K65" s="28">
-        <v>2017</v>
-      </c>
-      <c r="L65" s="29">
-        <f t="shared" si="13"/>
         <v>5.8123863373048987</v>
       </c>
-      <c r="M65" s="36">
-        <f t="shared" si="14"/>
+      <c r="M65" s="33">
+        <f t="shared" si="12"/>
         <v>1.3905065498909688</v>
       </c>
     </row>
@@ -9210,22 +9219,22 @@
         <v>2019</v>
       </c>
       <c r="H66">
+        <f t="shared" si="9"/>
+        <v>5.0481025000000002E-3</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="8"/>
+        <v>2.5240512500000001E-3</v>
+      </c>
+      <c r="K66" s="27">
+        <v>2018</v>
+      </c>
+      <c r="L66" s="38">
         <f t="shared" si="11"/>
-        <v>5.0481025000000002E-3</v>
-      </c>
-      <c r="I66">
-        <f t="shared" si="10"/>
-        <v>2.5240512500000001E-3</v>
-      </c>
-      <c r="K66" s="28">
-        <v>2018</v>
-      </c>
-      <c r="L66" s="29">
-        <f t="shared" si="13"/>
         <v>4.2476670629228757</v>
       </c>
-      <c r="M66" s="36">
-        <f t="shared" si="14"/>
+      <c r="M66" s="33">
+        <f t="shared" si="12"/>
         <v>1.0161762364008808</v>
       </c>
     </row>
@@ -9256,18 +9265,18 @@
         <v>5.0922496000000012E-3</v>
       </c>
       <c r="I67">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>2.5461248000000006E-3</v>
       </c>
-      <c r="K67" s="28">
+      <c r="K67" s="27">
         <v>2019</v>
       </c>
-      <c r="L67" s="29">
-        <f t="shared" si="13"/>
+      <c r="L67" s="38">
+        <f t="shared" si="11"/>
         <v>4.3089646422848977</v>
       </c>
-      <c r="M67" s="36">
-        <f t="shared" si="14"/>
+      <c r="M67" s="33">
+        <f t="shared" si="12"/>
         <v>1.0308405550901432</v>
       </c>
     </row>
@@ -9290,15 +9299,15 @@
       <c r="F68" t="s">
         <v>21</v>
       </c>
-      <c r="K68" s="30">
+      <c r="K68" s="28">
         <v>2020</v>
       </c>
-      <c r="L68" s="31">
-        <f t="shared" si="13"/>
+      <c r="L68" s="37">
+        <f t="shared" si="11"/>
         <v>6.0854442221906488</v>
       </c>
-      <c r="M68" s="37">
-        <f t="shared" si="14"/>
+      <c r="M68" s="34">
+        <f t="shared" si="12"/>
         <v>1.4558306277135495</v>
       </c>
     </row>
@@ -9385,7 +9394,7 @@
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A76" s="32" t="s">
+      <c r="A76" s="29" t="s">
         <v>20</v>
       </c>
     </row>
@@ -9418,10 +9427,10 @@
       </c>
       <c r="J79" s="24"/>
       <c r="K79" s="25"/>
-      <c r="L79" s="26" t="s">
+      <c r="L79" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="M79" s="27" t="s">
+      <c r="M79" s="26" t="s">
         <v>38</v>
       </c>
       <c r="N79" s="24"/>
@@ -9453,17 +9462,17 @@
         <v>8.7497315999999995E-3</v>
       </c>
       <c r="I80">
-        <f t="shared" ref="I80:I84" si="15">H80/2</f>
+        <f t="shared" ref="I80:I84" si="13">H80/2</f>
         <v>4.3748657999999998E-3</v>
       </c>
-      <c r="K80" s="28">
+      <c r="K80" s="27">
         <v>2008</v>
       </c>
       <c r="L80" s="38">
         <f>EXP(B80+I80)</f>
         <v>0.3203294971980486</v>
       </c>
-      <c r="M80" s="36">
+      <c r="M80" s="33">
         <f>L80/AVERAGE($L$80:$L$92)</f>
         <v>0.48807561114279352</v>
       </c>
@@ -9491,21 +9500,21 @@
         <v>2009</v>
       </c>
       <c r="H81">
-        <f t="shared" ref="H81:H84" si="16">C81^2</f>
+        <f t="shared" ref="H81:H84" si="14">C81^2</f>
         <v>1.21E-2</v>
       </c>
       <c r="I81">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>6.0499999999999998E-3</v>
       </c>
-      <c r="K81" s="28">
+      <c r="K81" s="27">
         <v>2009</v>
       </c>
       <c r="L81" s="38">
         <f>EXP($B$80+$I$80+B81+I81)</f>
         <v>0.39065708111865749</v>
       </c>
-      <c r="M81" s="36">
+      <c r="M81" s="33">
         <f>L81/AVERAGE($L$56:$L$68)</f>
         <v>9.3457523043565999E-2</v>
       </c>
@@ -9530,21 +9539,21 @@
         <v>2010</v>
       </c>
       <c r="H82">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>1.2452328099999998E-2</v>
       </c>
       <c r="I82">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>6.2261640499999991E-3</v>
       </c>
-      <c r="K82" s="28">
+      <c r="K82" s="27">
         <v>2010</v>
       </c>
       <c r="L82" s="38">
-        <f t="shared" ref="L82:L83" si="17">EXP($B$80+$I$80+B82+I82)</f>
+        <f t="shared" ref="L82:L83" si="15">EXP($B$80+$I$80+B82+I82)</f>
         <v>0.34500755275393963</v>
       </c>
-      <c r="M82" s="36">
+      <c r="M82" s="33">
         <f>L82/AVERAGE($L$56:$L$68)</f>
         <v>8.2536712810568583E-2</v>
       </c>
@@ -9572,21 +9581,21 @@
         <v>2011</v>
       </c>
       <c r="H83">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>2.0629576900000002E-2</v>
       </c>
       <c r="I83">
+        <f t="shared" si="13"/>
+        <v>1.0314788450000001E-2</v>
+      </c>
+      <c r="K83" s="27">
+        <v>2011</v>
+      </c>
+      <c r="L83" s="38">
         <f t="shared" si="15"/>
-        <v>1.0314788450000001E-2</v>
-      </c>
-      <c r="K83" s="28">
-        <v>2011</v>
-      </c>
-      <c r="L83" s="38">
-        <f t="shared" si="17"/>
         <v>0.16385222150766598</v>
       </c>
-      <c r="M83" s="36">
+      <c r="M83" s="33">
         <f>L83/AVERAGE($L$56:$L$68)</f>
         <v>3.9198630992281859E-2</v>
       </c>
@@ -9614,21 +9623,21 @@
         <v>2012</v>
       </c>
       <c r="H84">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>9.6353855999999991E-3</v>
       </c>
       <c r="I84">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>4.8176927999999996E-3</v>
       </c>
-      <c r="K84" s="28">
+      <c r="K84" s="27">
         <v>2012</v>
       </c>
       <c r="L84" s="38">
         <f>EXP($B$80+$I$80+B84+I84)</f>
         <v>2.194079417100145</v>
       </c>
-      <c r="M84" s="36">
+      <c r="M84" s="33">
         <f>L84/AVERAGE($L$56:$L$68)</f>
         <v>0.52489315462009545</v>
       </c>
@@ -9653,18 +9662,18 @@
         <v>2014</v>
       </c>
       <c r="H85">
-        <f t="shared" ref="H85:H91" si="18">C85^2</f>
+        <f t="shared" ref="H85:H91" si="16">C85^2</f>
         <v>1.59820164E-2</v>
       </c>
       <c r="I85">
-        <f t="shared" ref="I85:I91" si="19">H85/2</f>
+        <f t="shared" ref="I85:I91" si="17">H85/2</f>
         <v>7.9910082E-3</v>
       </c>
-      <c r="K85" s="28">
+      <c r="K85" s="27">
         <v>2013</v>
       </c>
       <c r="L85" s="38"/>
-      <c r="M85" s="36"/>
+      <c r="M85" s="33"/>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
@@ -9689,22 +9698,22 @@
         <v>2015</v>
       </c>
       <c r="H86">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>1.3572250000000001E-2</v>
       </c>
       <c r="I86">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>6.7861250000000005E-3</v>
       </c>
-      <c r="K86" s="28">
+      <c r="K86" s="27">
         <v>2014</v>
       </c>
       <c r="L86" s="38">
         <f>EXP($B$80+$I$80+B85+I85)</f>
         <v>0.29672362588144763</v>
       </c>
-      <c r="M86" s="36">
-        <f t="shared" ref="M86:M92" si="20">L86/AVERAGE($L$56:$L$68)</f>
+      <c r="M86" s="33">
+        <f t="shared" ref="M86:M92" si="18">L86/AVERAGE($L$56:$L$68)</f>
         <v>7.0985671177333315E-2</v>
       </c>
     </row>
@@ -9731,22 +9740,22 @@
         <v>2016</v>
       </c>
       <c r="H87">
+        <f t="shared" si="16"/>
+        <v>1.0424409999999999E-2</v>
+      </c>
+      <c r="I87">
+        <f t="shared" si="17"/>
+        <v>5.2122049999999993E-3</v>
+      </c>
+      <c r="K87" s="27">
+        <v>2015</v>
+      </c>
+      <c r="L87" s="38">
+        <f t="shared" ref="L87:L92" si="19">EXP($B$80+$I$80+B86+I86)</f>
+        <v>0.44856171259042121</v>
+      </c>
+      <c r="M87" s="33">
         <f t="shared" si="18"/>
-        <v>1.0424409999999999E-2</v>
-      </c>
-      <c r="I87">
-        <f t="shared" si="19"/>
-        <v>5.2122049999999993E-3</v>
-      </c>
-      <c r="K87" s="28">
-        <v>2015</v>
-      </c>
-      <c r="L87" s="38">
-        <f t="shared" ref="L87:L92" si="21">EXP($B$80+$I$80+B86+I86)</f>
-        <v>0.44856171259042121</v>
-      </c>
-      <c r="M87" s="36">
-        <f t="shared" si="20"/>
         <v>0.10731014134144817</v>
       </c>
     </row>
@@ -9773,22 +9782,22 @@
         <v>2017</v>
       </c>
       <c r="H88">
+        <f t="shared" si="16"/>
+        <v>1.2638256400000001E-2</v>
+      </c>
+      <c r="I88">
+        <f t="shared" si="17"/>
+        <v>6.3191282000000003E-3</v>
+      </c>
+      <c r="K88" s="27">
+        <v>2016</v>
+      </c>
+      <c r="L88" s="38">
+        <f t="shared" si="19"/>
+        <v>1.148925400073296</v>
+      </c>
+      <c r="M88" s="33">
         <f t="shared" si="18"/>
-        <v>1.2638256400000001E-2</v>
-      </c>
-      <c r="I88">
-        <f t="shared" si="19"/>
-        <v>6.3191282000000003E-3</v>
-      </c>
-      <c r="K88" s="28">
-        <v>2016</v>
-      </c>
-      <c r="L88" s="38">
-        <f t="shared" si="21"/>
-        <v>1.148925400073296</v>
-      </c>
-      <c r="M88" s="36">
-        <f t="shared" si="20"/>
         <v>0.27485927490477063</v>
       </c>
     </row>
@@ -9812,22 +9821,22 @@
         <v>2018</v>
       </c>
       <c r="H89">
+        <f t="shared" si="16"/>
+        <v>1.2566410000000002E-2</v>
+      </c>
+      <c r="I89">
+        <f t="shared" si="17"/>
+        <v>6.2832050000000009E-3</v>
+      </c>
+      <c r="K89" s="27">
+        <v>2017</v>
+      </c>
+      <c r="L89" s="38">
+        <f t="shared" si="19"/>
+        <v>0.77669619228149478</v>
+      </c>
+      <c r="M89" s="33">
         <f t="shared" si="18"/>
-        <v>1.2566410000000002E-2</v>
-      </c>
-      <c r="I89">
-        <f t="shared" si="19"/>
-        <v>6.2832050000000009E-3</v>
-      </c>
-      <c r="K89" s="28">
-        <v>2017</v>
-      </c>
-      <c r="L89" s="38">
-        <f t="shared" si="21"/>
-        <v>0.77669619228149478</v>
-      </c>
-      <c r="M89" s="36">
-        <f t="shared" si="20"/>
         <v>0.18581028169293567</v>
       </c>
     </row>
@@ -9854,22 +9863,22 @@
         <v>2019</v>
       </c>
       <c r="H90">
+        <f t="shared" si="16"/>
+        <v>1.11218116E-2</v>
+      </c>
+      <c r="I90">
+        <f t="shared" si="17"/>
+        <v>5.5609057999999999E-3</v>
+      </c>
+      <c r="K90" s="27">
+        <v>2018</v>
+      </c>
+      <c r="L90" s="38">
+        <f t="shared" si="19"/>
+        <v>0.31225287295566323</v>
+      </c>
+      <c r="M90" s="33">
         <f t="shared" si="18"/>
-        <v>1.11218116E-2</v>
-      </c>
-      <c r="I90">
-        <f t="shared" si="19"/>
-        <v>5.5609057999999999E-3</v>
-      </c>
-      <c r="K90" s="28">
-        <v>2018</v>
-      </c>
-      <c r="L90" s="38">
-        <f t="shared" si="21"/>
-        <v>0.31225287295566323</v>
-      </c>
-      <c r="M90" s="36">
-        <f t="shared" si="20"/>
         <v>7.4700757979630161E-2</v>
       </c>
     </row>
@@ -9896,22 +9905,22 @@
         <v>2020</v>
       </c>
       <c r="H91">
+        <f t="shared" si="16"/>
+        <v>1.04530176E-2</v>
+      </c>
+      <c r="I91">
+        <f t="shared" si="17"/>
+        <v>5.2265087999999998E-3</v>
+      </c>
+      <c r="K91" s="27">
+        <v>2019</v>
+      </c>
+      <c r="L91" s="38">
+        <f t="shared" si="19"/>
+        <v>0.55421962908814715</v>
+      </c>
+      <c r="M91" s="33">
         <f t="shared" si="18"/>
-        <v>1.04530176E-2</v>
-      </c>
-      <c r="I91">
-        <f t="shared" si="19"/>
-        <v>5.2265087999999998E-3</v>
-      </c>
-      <c r="K91" s="28">
-        <v>2019</v>
-      </c>
-      <c r="L91" s="38">
-        <f t="shared" si="21"/>
-        <v>0.55421962908814715</v>
-      </c>
-      <c r="M91" s="36">
-        <f t="shared" si="20"/>
         <v>0.13258685496851313</v>
       </c>
     </row>
@@ -9931,15 +9940,15 @@
       <c r="E92">
         <v>0.27187</v>
       </c>
-      <c r="K92" s="30">
+      <c r="K92" s="28">
         <v>2020</v>
       </c>
-      <c r="L92" s="31">
-        <f t="shared" si="21"/>
+      <c r="L92" s="37">
+        <f t="shared" si="19"/>
         <v>0.92442937344482978</v>
       </c>
-      <c r="M92" s="37">
-        <f t="shared" si="20"/>
+      <c r="M92" s="34">
+        <f t="shared" si="18"/>
         <v>0.22115272868848379</v>
       </c>
     </row>
@@ -10038,8 +10047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC2DBA19-5AF2-41C9-920C-E4F4CE48DF6B}">
   <dimension ref="A1:N99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J99" sqref="J99"/>
+    <sheetView topLeftCell="E33" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10048,7 +10057,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="29" t="s">
         <v>22</v>
       </c>
     </row>
@@ -10087,13 +10096,13 @@
       </c>
       <c r="J6" s="24"/>
       <c r="K6" s="25"/>
-      <c r="L6" s="26" t="s">
+      <c r="L6" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="M6" s="27" t="s">
+      <c r="M6" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="N6" s="33" t="s">
+      <c r="N6" s="30" t="s">
         <v>64</v>
       </c>
     </row>
@@ -10127,18 +10136,18 @@
         <f t="shared" ref="I7:I18" si="0">H7/2</f>
         <v>1.3645088E-3</v>
       </c>
-      <c r="K7" s="28">
+      <c r="K7" s="27">
         <v>2006</v>
       </c>
-      <c r="L7" s="29">
-        <f>(B7+I7)</f>
-        <v>-0.16197549120000002</v>
-      </c>
-      <c r="M7" s="36">
+      <c r="L7" s="36">
+        <f>EXP(B7+I7)</f>
+        <v>0.85046204808905101</v>
+      </c>
+      <c r="M7" s="33">
         <f>L7/AVERAGE($L$7:$L$21)</f>
-        <v>-0.22255980611592036</v>
-      </c>
-      <c r="N7" s="34">
+        <v>0.36438776132468909</v>
+      </c>
+      <c r="N7" s="31">
         <v>1.21</v>
       </c>
     </row>
@@ -10172,18 +10181,18 @@
         <f t="shared" si="0"/>
         <v>2.1040584499999997E-3</v>
       </c>
-      <c r="K8" s="28">
+      <c r="K8" s="27">
         <v>2007</v>
       </c>
-      <c r="L8" s="29">
-        <f>($B$7+$I$7+B8+I8)</f>
-        <v>0.24757856724999996</v>
-      </c>
-      <c r="M8" s="36">
+      <c r="L8" s="36">
+        <f>EXP($B$7+$I$7+B8+I8)</f>
+        <v>1.2809199967920037</v>
+      </c>
+      <c r="M8" s="33">
         <f t="shared" ref="M8:M20" si="2">L8/AVERAGE($L$7:$L$21)</f>
-        <v>0.34018132939372331</v>
-      </c>
-      <c r="N8" s="34">
+        <v>0.5488211627030688</v>
+      </c>
+      <c r="N8" s="31">
         <v>1.25</v>
       </c>
     </row>
@@ -10217,18 +10226,18 @@
         <f t="shared" si="0"/>
         <v>2.0756124500000001E-3</v>
       </c>
-      <c r="K9" s="28">
+      <c r="K9" s="27">
         <v>2008</v>
       </c>
-      <c r="L9" s="29">
-        <f t="shared" ref="L9:L21" si="3">($B$7+$I$7+B9+I9)</f>
-        <v>0.26696012125000002</v>
-      </c>
-      <c r="M9" s="36">
+      <c r="L9" s="36">
+        <f t="shared" ref="L9:L21" si="3">EXP($B$7+$I$7+B9+I9)</f>
+        <v>1.3059883641086991</v>
+      </c>
+      <c r="M9" s="33">
         <f t="shared" si="2"/>
-        <v>0.36681224045630545</v>
-      </c>
-      <c r="N9" s="34">
+        <v>0.55956191976227054</v>
+      </c>
+      <c r="N9" s="31">
         <v>1.26</v>
       </c>
     </row>
@@ -10262,18 +10271,18 @@
         <f t="shared" si="0"/>
         <v>1.6843208000000001E-3</v>
       </c>
-      <c r="K10" s="28">
+      <c r="K10" s="27">
         <v>2009</v>
       </c>
-      <c r="L10" s="29">
+      <c r="L10" s="36">
         <f t="shared" si="3"/>
-        <v>0.2243288296</v>
-      </c>
-      <c r="M10" s="36">
+        <v>1.2514824762571373</v>
+      </c>
+      <c r="M10" s="33">
         <f t="shared" si="2"/>
-        <v>0.3082354030977455</v>
-      </c>
-      <c r="N10" s="34">
+        <v>0.53620840446094398</v>
+      </c>
+      <c r="N10" s="31">
         <v>1.75</v>
       </c>
     </row>
@@ -10307,18 +10316,18 @@
         <f t="shared" si="0"/>
         <v>1.4927648E-3</v>
       </c>
-      <c r="K11" s="28">
+      <c r="K11" s="27">
         <v>2010</v>
       </c>
-      <c r="L11" s="29">
+      <c r="L11" s="36">
         <f t="shared" si="3"/>
-        <v>0.45269727359999995</v>
-      </c>
-      <c r="M11" s="36">
+        <v>1.5725480626363486</v>
+      </c>
+      <c r="M11" s="33">
         <f t="shared" si="2"/>
-        <v>0.62202137308055727</v>
-      </c>
-      <c r="N11" s="34">
+        <v>0.67377170963369781</v>
+      </c>
+      <c r="N11" s="31">
         <v>2.27</v>
       </c>
     </row>
@@ -10349,18 +10358,18 @@
         <f t="shared" si="0"/>
         <v>1.8568418E-3</v>
       </c>
-      <c r="K12" s="28">
+      <c r="K12" s="27">
         <v>2011</v>
       </c>
-      <c r="L12" s="29">
+      <c r="L12" s="36">
         <f t="shared" si="3"/>
-        <v>-6.7398649400000024E-2</v>
-      </c>
-      <c r="M12" s="36">
+        <v>0.93482246063224628</v>
+      </c>
+      <c r="M12" s="33">
         <f t="shared" si="2"/>
-        <v>-9.2608025027794416E-2</v>
-      </c>
-      <c r="N12" s="34">
+        <v>0.40053270387693263</v>
+      </c>
+      <c r="N12" s="31">
         <v>1.31</v>
       </c>
     </row>
@@ -10394,18 +10403,18 @@
         <f t="shared" si="0"/>
         <v>1.5384604499999999E-3</v>
       </c>
-      <c r="K13" s="28">
+      <c r="K13" s="27">
         <v>2012</v>
       </c>
-      <c r="L13" s="29">
+      <c r="L13" s="36">
         <f t="shared" si="3"/>
-        <v>1.1774729692499999</v>
-      </c>
-      <c r="M13" s="36">
+        <v>3.2461606814884179</v>
+      </c>
+      <c r="M13" s="33">
         <f t="shared" si="2"/>
-        <v>1.6178877051185445</v>
-      </c>
-      <c r="N13" s="34">
+        <v>1.3908453954948681</v>
+      </c>
+      <c r="N13" s="31">
         <v>3.18</v>
       </c>
     </row>
@@ -10439,18 +10448,18 @@
         <f t="shared" si="0"/>
         <v>1.4504498E-3</v>
       </c>
-      <c r="K14" s="28">
+      <c r="K14" s="27">
         <v>2013</v>
       </c>
-      <c r="L14" s="29">
+      <c r="L14" s="36">
         <f t="shared" si="3"/>
-        <v>1.4580549586</v>
-      </c>
-      <c r="M14" s="36">
+        <v>4.2975923986405551</v>
+      </c>
+      <c r="M14" s="33">
         <f t="shared" si="2"/>
-        <v>2.0034168533046079</v>
-      </c>
-      <c r="N14" s="34">
+        <v>1.8413403358155018</v>
+      </c>
+      <c r="N14" s="31">
         <v>4.09</v>
       </c>
     </row>
@@ -10484,18 +10493,18 @@
         <f t="shared" si="0"/>
         <v>1.4553012499999999E-3</v>
       </c>
-      <c r="K15" s="28">
+      <c r="K15" s="27">
         <v>2014</v>
       </c>
-      <c r="L15" s="29">
+      <c r="L15" s="36">
         <f t="shared" si="3"/>
-        <v>1.4212398100500001</v>
-      </c>
-      <c r="M15" s="36">
+        <v>4.1422528647095564</v>
+      </c>
+      <c r="M15" s="33">
         <f t="shared" si="2"/>
-        <v>1.9528315933821687</v>
-      </c>
-      <c r="N15" s="34">
+        <v>1.7747837797157637</v>
+      </c>
+      <c r="N15" s="31">
         <v>4.16</v>
       </c>
     </row>
@@ -10529,18 +10538,18 @@
         <f t="shared" si="0"/>
         <v>1.5814688E-3</v>
       </c>
-      <c r="K16" s="28">
+      <c r="K16" s="27">
         <v>2015</v>
       </c>
-      <c r="L16" s="29">
+      <c r="L16" s="36">
         <f t="shared" si="3"/>
-        <v>1.0063159775999999</v>
-      </c>
-      <c r="M16" s="36">
+        <v>2.7355047681947258</v>
+      </c>
+      <c r="M16" s="33">
         <f t="shared" si="2"/>
-        <v>1.3827122066848148</v>
-      </c>
-      <c r="N16" s="34">
+        <v>1.1720504881025759</v>
+      </c>
+      <c r="N16" s="31">
         <v>2.86</v>
       </c>
     </row>
@@ -10574,18 +10583,18 @@
         <f t="shared" si="0"/>
         <v>1.6091464500000003E-3</v>
       </c>
-      <c r="K17" s="28">
+      <c r="K17" s="27">
         <v>2016</v>
       </c>
-      <c r="L17" s="29">
+      <c r="L17" s="36">
         <f t="shared" si="3"/>
-        <v>1.01790365525</v>
-      </c>
-      <c r="M17" s="36">
+        <v>2.7673872810501194</v>
+      </c>
+      <c r="M17" s="33">
         <f t="shared" si="2"/>
-        <v>1.3986340678998146</v>
-      </c>
-      <c r="N17" s="34">
+        <v>1.1857108242820524</v>
+      </c>
+      <c r="N17" s="31">
         <v>2.76</v>
       </c>
     </row>
@@ -10619,18 +10628,18 @@
         <f t="shared" si="0"/>
         <v>1.5618460500000002E-3</v>
       </c>
-      <c r="K18" s="28">
+      <c r="K18" s="27">
         <v>2017</v>
       </c>
-      <c r="L18" s="29">
+      <c r="L18" s="36">
         <f t="shared" si="3"/>
-        <v>0.98599635484999992</v>
-      </c>
-      <c r="M18" s="36">
+        <v>2.6804812648837357</v>
+      </c>
+      <c r="M18" s="33">
         <f t="shared" si="2"/>
-        <v>1.3547923574157381</v>
-      </c>
-      <c r="N18" s="34">
+        <v>1.148475196016604</v>
+      </c>
+      <c r="N18" s="31">
         <v>3.09</v>
       </c>
     </row>
@@ -10664,18 +10673,18 @@
         <f t="shared" ref="I19:I21" si="4">H19/2</f>
         <v>1.6583040500000002E-3</v>
       </c>
-      <c r="K19" s="28">
+      <c r="K19" s="27">
         <v>2018</v>
       </c>
-      <c r="L19" s="29">
+      <c r="L19" s="36">
         <f t="shared" si="3"/>
-        <v>0.77690281285000007</v>
-      </c>
-      <c r="M19" s="36">
+        <v>2.1747262897966491</v>
+      </c>
+      <c r="M19" s="33">
         <f t="shared" si="2"/>
-        <v>1.0674907550384336</v>
-      </c>
-      <c r="N19" s="34">
+        <v>0.93178013764815526</v>
+      </c>
+      <c r="N19" s="31">
         <v>2.4</v>
       </c>
     </row>
@@ -10709,18 +10718,18 @@
         <f t="shared" si="4"/>
         <v>1.6057444499999998E-3</v>
       </c>
-      <c r="K20" s="28">
+      <c r="K20" s="27">
         <v>2019</v>
       </c>
-      <c r="L20" s="29">
+      <c r="L20" s="36">
         <f t="shared" si="3"/>
-        <v>0.96595025324999995</v>
-      </c>
-      <c r="M20" s="36">
+        <v>2.6272830549181658</v>
+      </c>
+      <c r="M20" s="33">
         <f t="shared" si="2"/>
-        <v>1.3272483354626439</v>
-      </c>
-      <c r="N20" s="34">
+        <v>1.1256819665251865</v>
+      </c>
+      <c r="N20" s="31">
         <v>2.64</v>
       </c>
     </row>
@@ -10754,18 +10763,18 @@
         <f t="shared" si="4"/>
         <v>1.50975125E-3</v>
       </c>
-      <c r="K21" s="30">
+      <c r="K21" s="28">
         <v>2020</v>
       </c>
-      <c r="L21" s="31">
+      <c r="L21" s="37">
         <f t="shared" si="3"/>
-        <v>1.1447342600499999</v>
-      </c>
-      <c r="M21" s="37">
+        <v>3.1416063955763178</v>
+      </c>
+      <c r="M21" s="34">
         <f>L21/AVERAGE($L$7:$L$21)</f>
-        <v>1.5729036108086178</v>
-      </c>
-      <c r="N21" s="35">
+        <v>1.3460482146376898</v>
+      </c>
+      <c r="N21" s="32">
         <v>3.53</v>
       </c>
     </row>
@@ -10850,7 +10859,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="29" t="s">
         <v>24</v>
       </c>
       <c r="F28" s="14"/>
@@ -10884,13 +10893,13 @@
       </c>
       <c r="J31" s="24"/>
       <c r="K31" s="25"/>
-      <c r="L31" s="26" t="s">
+      <c r="L31" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="M31" s="27" t="s">
+      <c r="M31" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="N31" s="33" t="s">
+      <c r="N31" s="30" t="s">
         <v>64</v>
       </c>
     </row>
@@ -10924,18 +10933,18 @@
         <f t="shared" ref="I32:I43" si="6">H32/2</f>
         <v>8.9151304500000011E-3</v>
       </c>
-      <c r="K32" s="28">
+      <c r="K32" s="27">
         <v>2006</v>
       </c>
-      <c r="L32" s="29">
-        <f>(B32+I32)</f>
-        <v>-2.5190748695499998</v>
-      </c>
-      <c r="M32" s="36">
+      <c r="L32" s="36">
+        <f>EXP(B32+I32)</f>
+        <v>8.0534076823686698E-2</v>
+      </c>
+      <c r="M32" s="33">
         <f>L32/AVERAGE($L$32:$L$46)</f>
-        <v>1.5418167457242424</v>
-      </c>
-      <c r="N32" s="34">
+        <v>0.29566268665885315</v>
+      </c>
+      <c r="N32" s="31">
         <v>0.218</v>
       </c>
     </row>
@@ -10969,18 +10978,18 @@
         <f t="shared" si="6"/>
         <v>1.4260227200000001E-2</v>
       </c>
-      <c r="K33" s="28">
+      <c r="K33" s="27">
         <v>2007</v>
       </c>
-      <c r="L33" s="29">
-        <f>($B$32+$I$32+B33+I33)</f>
-        <v>-2.0285746423500002</v>
-      </c>
-      <c r="M33" s="36">
+      <c r="L33" s="36">
+        <f>EXP($B$32+$I$32+B33+I33)</f>
+        <v>0.13152285471522876</v>
+      </c>
+      <c r="M33" s="33">
         <f t="shared" ref="M33:M45" si="7">L33/AVERAGE($L$32:$L$46)</f>
-        <v>1.241602777008973</v>
-      </c>
-      <c r="N33" s="34">
+        <v>0.48285647661027475</v>
+      </c>
+      <c r="N33" s="31">
         <v>0.16900000000000001</v>
       </c>
     </row>
@@ -11011,18 +11020,18 @@
         <f t="shared" si="6"/>
         <v>1.5652112450000002E-2</v>
       </c>
-      <c r="K34" s="28">
+      <c r="K34" s="27">
         <v>2008</v>
       </c>
-      <c r="L34" s="29">
-        <f t="shared" ref="L34:L46" si="8">($B$32+$I$32+B34+I34)</f>
-        <v>-2.2184427570999996</v>
-      </c>
-      <c r="M34" s="36">
+      <c r="L34" s="36">
+        <f t="shared" ref="L34:L46" si="8">EXP($B$32+$I$32+B34+I34)</f>
+        <v>0.1087783713457752</v>
+      </c>
+      <c r="M34" s="33">
         <f t="shared" si="7"/>
-        <v>1.3578128358441579</v>
-      </c>
-      <c r="N34" s="34">
+        <v>0.39935523930916778</v>
+      </c>
+      <c r="N34" s="31">
         <v>0.13900000000000001</v>
       </c>
     </row>
@@ -11056,18 +11065,18 @@
         <f t="shared" si="6"/>
         <v>8.9994528000000001E-3</v>
       </c>
-      <c r="K35" s="28">
+      <c r="K35" s="27">
         <v>2009</v>
       </c>
-      <c r="L35" s="29">
+      <c r="L35" s="36">
         <f t="shared" si="8"/>
-        <v>-2.02914541675</v>
-      </c>
-      <c r="M35" s="36">
+        <v>0.13144780625664931</v>
+      </c>
+      <c r="M35" s="33">
         <f>L35/AVERAGE($L$32:$L$46)</f>
-        <v>1.2419521233259834</v>
-      </c>
-      <c r="N35" s="34">
+        <v>0.48258095313290528</v>
+      </c>
+      <c r="N35" s="31">
         <v>0.34599999999999997</v>
       </c>
     </row>
@@ -11098,18 +11107,18 @@
         <f t="shared" si="6"/>
         <v>1.0531358450000002E-2</v>
       </c>
-      <c r="K36" s="28">
+      <c r="K36" s="27">
         <v>2010</v>
       </c>
-      <c r="L36" s="29">
+      <c r="L36" s="36">
         <f t="shared" si="8"/>
-        <v>-2.4340535110999997</v>
-      </c>
-      <c r="M36" s="36">
+        <v>8.7680696592522728E-2</v>
+      </c>
+      <c r="M36" s="33">
         <f t="shared" si="7"/>
-        <v>1.4897788504687313</v>
-      </c>
-      <c r="N36" s="34">
+        <v>0.32189988816063853</v>
+      </c>
+      <c r="N36" s="31">
         <v>0.222</v>
       </c>
     </row>
@@ -11143,18 +11152,18 @@
         <f t="shared" si="6"/>
         <v>1.2952451250000002E-2</v>
       </c>
-      <c r="K37" s="28">
+      <c r="K37" s="27">
         <v>2011</v>
       </c>
-      <c r="L37" s="29">
+      <c r="L37" s="36">
         <f t="shared" si="8"/>
-        <v>-2.8387424182999998</v>
-      </c>
-      <c r="M37" s="36">
+        <v>5.8499187232639221E-2</v>
+      </c>
+      <c r="M37" s="33">
         <f t="shared" si="7"/>
-        <v>1.7374714226395878</v>
-      </c>
-      <c r="N37" s="34">
+        <v>0.21476656276109796</v>
+      </c>
+      <c r="N37" s="31">
         <v>0.154</v>
       </c>
     </row>
@@ -11188,18 +11197,18 @@
         <f t="shared" si="6"/>
         <v>8.2689799999999987E-3</v>
       </c>
-      <c r="K38" s="28">
+      <c r="K38" s="27">
         <v>2012</v>
       </c>
-      <c r="L38" s="29">
+      <c r="L38" s="36">
         <f t="shared" si="8"/>
-        <v>-6.7495889549999952E-2</v>
-      </c>
-      <c r="M38" s="36">
+        <v>0.9347315627754833</v>
+      </c>
+      <c r="M38" s="33">
         <f t="shared" si="7"/>
-        <v>4.1311313940555462E-2</v>
-      </c>
-      <c r="N38" s="34">
+        <v>3.4316559654626011</v>
+      </c>
+      <c r="N38" s="31">
         <v>1.19</v>
       </c>
     </row>
@@ -11233,18 +11242,18 @@
         <f t="shared" si="6"/>
         <v>1.0506700800000001E-2</v>
       </c>
-      <c r="K39" s="28">
+      <c r="K39" s="27">
         <v>2013</v>
       </c>
-      <c r="L39" s="29">
+      <c r="L39" s="36">
         <f t="shared" si="8"/>
-        <v>-1.22844816875</v>
-      </c>
-      <c r="M39" s="36">
+        <v>0.29274651856577544</v>
+      </c>
+      <c r="M39" s="33">
         <f t="shared" si="7"/>
-        <v>0.75187997813315333</v>
-      </c>
-      <c r="N39" s="34">
+        <v>1.0747527705405528</v>
+      </c>
+      <c r="N39" s="31">
         <v>0.36899999999999999</v>
       </c>
     </row>
@@ -11275,18 +11284,18 @@
         <f t="shared" si="6"/>
         <v>1.5936480449999998E-2</v>
       </c>
-      <c r="K40" s="28">
+      <c r="K40" s="27">
         <v>2014</v>
       </c>
-      <c r="L40" s="29">
+      <c r="L40" s="36">
         <f t="shared" si="8"/>
-        <v>-2.2378983890999997</v>
-      </c>
-      <c r="M40" s="36">
+        <v>0.1066824739985154</v>
+      </c>
+      <c r="M40" s="33">
         <f t="shared" si="7"/>
-        <v>1.3697207864885972</v>
-      </c>
-      <c r="N40" s="34">
+        <v>0.39166062523904366</v>
+      </c>
+      <c r="N40" s="31">
         <v>0.14799999999999999</v>
       </c>
     </row>
@@ -11320,18 +11329,18 @@
         <f t="shared" si="6"/>
         <v>1.2222661249999999E-2</v>
       </c>
-      <c r="K41" s="28">
+      <c r="K41" s="27">
         <v>2015</v>
       </c>
-      <c r="L41" s="29">
+      <c r="L41" s="36">
         <f t="shared" si="8"/>
-        <v>-1.7594322082999998</v>
-      </c>
-      <c r="M41" s="36">
+        <v>0.17214257720655585</v>
+      </c>
+      <c r="M41" s="33">
         <f t="shared" si="7"/>
-        <v>1.0768723369496818</v>
-      </c>
-      <c r="N41" s="34">
+        <v>0.63198261993735028</v>
+      </c>
+      <c r="N41" s="31">
         <v>0.245</v>
       </c>
     </row>
@@ -11365,18 +11374,18 @@
         <f t="shared" si="6"/>
         <v>9.9334512499999993E-3</v>
       </c>
-      <c r="K42" s="28">
+      <c r="K42" s="27">
         <v>2016</v>
       </c>
-      <c r="L42" s="29">
+      <c r="L42" s="36">
         <f t="shared" si="8"/>
-        <v>-1.0348814182999999</v>
-      </c>
-      <c r="M42" s="36">
+        <v>0.35526850677071431</v>
+      </c>
+      <c r="M42" s="33">
         <f t="shared" si="7"/>
-        <v>0.63340614439888687</v>
-      </c>
-      <c r="N42" s="34">
+        <v>1.304288139132354</v>
+      </c>
+      <c r="N42" s="31">
         <v>0.46700000000000003</v>
       </c>
     </row>
@@ -11410,18 +11419,18 @@
         <f t="shared" si="6"/>
         <v>9.8771512500000005E-3</v>
       </c>
-      <c r="K43" s="28">
+      <c r="K43" s="27">
         <v>2017</v>
       </c>
-      <c r="L43" s="29">
+      <c r="L43" s="36">
         <f t="shared" si="8"/>
-        <v>-1.1970077182999999</v>
-      </c>
-      <c r="M43" s="36">
+        <v>0.30209681959540247</v>
+      </c>
+      <c r="M43" s="33">
         <f t="shared" si="7"/>
-        <v>0.73263663861082196</v>
-      </c>
-      <c r="N43" s="34">
+        <v>1.1090802904243526</v>
+      </c>
+      <c r="N43" s="31">
         <v>0.48199999999999998</v>
       </c>
     </row>
@@ -11455,18 +11464,18 @@
         <f t="shared" ref="I44:I45" si="10">H44/2</f>
         <v>1.2252385800000001E-2</v>
       </c>
-      <c r="K44" s="28">
+      <c r="K44" s="27">
         <v>2018</v>
       </c>
-      <c r="L44" s="29">
+      <c r="L44" s="36">
         <f t="shared" si="8"/>
-        <v>-1.8300224837499997</v>
-      </c>
-      <c r="M44" s="36">
+        <v>0.1604099611171641</v>
+      </c>
+      <c r="M44" s="33">
         <f t="shared" si="7"/>
-        <v>1.1200775906282034</v>
-      </c>
-      <c r="N44" s="34">
+        <v>0.58890896799593784</v>
+      </c>
+      <c r="N44" s="31">
         <v>0.24099999999999999</v>
       </c>
     </row>
@@ -11500,18 +11509,18 @@
         <f t="shared" si="10"/>
         <v>8.8205761999999993E-3</v>
       </c>
-      <c r="K45" s="28">
+      <c r="K45" s="27">
         <v>2019</v>
       </c>
-      <c r="L45" s="29">
+      <c r="L45" s="36">
         <f t="shared" si="8"/>
-        <v>-0.56276429334999989</v>
-      </c>
-      <c r="M45" s="36">
+        <v>0.56963225481759228</v>
+      </c>
+      <c r="M45" s="33">
         <f t="shared" si="7"/>
-        <v>0.34444367726859165</v>
-      </c>
-      <c r="N45" s="34">
+        <v>2.0912762585660429</v>
+      </c>
+      <c r="N45" s="31">
         <v>0.77600000000000002</v>
       </c>
     </row>
@@ -11545,18 +11554,18 @@
         <f>H46/2</f>
         <v>8.6671778000000001E-3</v>
       </c>
-      <c r="K46" s="30">
+      <c r="K46" s="28">
         <v>2020</v>
       </c>
-      <c r="L46" s="31">
+      <c r="L46" s="37">
         <f t="shared" si="8"/>
-        <v>-0.52154769174999971</v>
-      </c>
-      <c r="M46" s="37">
+        <v>0.59360112509802088</v>
+      </c>
+      <c r="M46" s="34">
         <f>L46/AVERAGE($L$32:$L$46)</f>
-        <v>0.31921677856983366</v>
-      </c>
-      <c r="N46" s="35">
+        <v>2.1792725560688253</v>
+      </c>
+      <c r="N46" s="32">
         <v>0.90600000000000003</v>
       </c>
     </row>
@@ -11647,7 +11656,7 @@
       <c r="E52" s="14"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A53" s="32" t="s">
+      <c r="A53" s="29" t="s">
         <v>26</v>
       </c>
       <c r="E53" s="14"/>
@@ -11681,10 +11690,10 @@
       </c>
       <c r="J56" s="24"/>
       <c r="K56" s="25"/>
-      <c r="L56" s="26" t="s">
+      <c r="L56" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="M56" s="27" t="s">
+      <c r="M56" s="26" t="s">
         <v>38</v>
       </c>
       <c r="N56" s="24"/>
@@ -11719,14 +11728,14 @@
         <f t="shared" ref="I57:I68" si="11">H57/2</f>
         <v>4.4490744499999998E-3</v>
       </c>
-      <c r="K57" s="28">
+      <c r="K57" s="27">
         <v>2006</v>
       </c>
-      <c r="L57" s="29">
+      <c r="L57" s="38">
         <f>EXP(B57+I57)</f>
         <v>0.84527697391665213</v>
       </c>
-      <c r="M57" s="36">
+      <c r="M57" s="33">
         <f>L57/AVERAGE($L$57:$L$71)</f>
         <v>0.33812056503325971</v>
       </c>
@@ -11761,14 +11770,14 @@
         <f t="shared" si="11"/>
         <v>6.3123848000000001E-3</v>
       </c>
-      <c r="K58" s="28">
+      <c r="K58" s="27">
         <v>2007</v>
       </c>
-      <c r="L58" s="29">
+      <c r="L58" s="38">
         <f>EXP($B$57+$I$57+B58+I58)</f>
         <v>1.274318415060075</v>
       </c>
-      <c r="M58" s="36">
+      <c r="M58" s="33">
         <f t="shared" ref="M58:M71" si="13">L58/AVERAGE($L$57:$L$71)</f>
         <v>0.50974210327286928</v>
       </c>
@@ -11803,14 +11812,14 @@
         <f t="shared" si="11"/>
         <v>6.2540927999999996E-3</v>
       </c>
-      <c r="K59" s="28">
+      <c r="K59" s="27">
         <v>2008</v>
       </c>
-      <c r="L59" s="29">
+      <c r="L59" s="38">
         <f t="shared" ref="L59:L71" si="14">EXP($B$57+$I$57+B59+I59)</f>
         <v>1.2959748180832642</v>
       </c>
-      <c r="M59" s="36">
+      <c r="M59" s="33">
         <f t="shared" si="13"/>
         <v>0.51840491493430552</v>
       </c>
@@ -11845,14 +11854,14 @@
         <f t="shared" si="11"/>
         <v>5.604228450000001E-3</v>
       </c>
-      <c r="K60" s="28">
+      <c r="K60" s="27">
         <v>2009</v>
       </c>
-      <c r="L60" s="29">
+      <c r="L60" s="38">
         <f t="shared" si="14"/>
         <v>1.3560055777571873</v>
       </c>
-      <c r="M60" s="36">
+      <c r="M60" s="33">
         <f t="shared" si="13"/>
         <v>0.54241791304813347</v>
       </c>
@@ -11887,14 +11896,14 @@
         <f t="shared" si="11"/>
         <v>5.2040402000000001E-3</v>
       </c>
-      <c r="K61" s="28">
+      <c r="K61" s="27">
         <v>2010</v>
       </c>
-      <c r="L61" s="29">
+      <c r="L61" s="38">
         <f t="shared" si="14"/>
         <v>1.8468530094598747</v>
       </c>
-      <c r="M61" s="36">
+      <c r="M61" s="33">
         <f t="shared" si="13"/>
         <v>0.7387625622859133</v>
       </c>
@@ -11926,14 +11935,14 @@
         <f t="shared" si="11"/>
         <v>5.6903112E-3</v>
       </c>
-      <c r="K62" s="28">
+      <c r="K62" s="27">
         <v>2011</v>
       </c>
-      <c r="L62" s="29">
+      <c r="L62" s="38">
         <f t="shared" si="14"/>
         <v>0.97498751387338378</v>
       </c>
-      <c r="M62" s="36">
+      <c r="M62" s="33">
         <f t="shared" si="13"/>
         <v>0.39000628109354823</v>
       </c>
@@ -11968,14 +11977,14 @@
         <f t="shared" si="11"/>
         <v>5.7566450000000003E-3</v>
       </c>
-      <c r="K63" s="28">
+      <c r="K63" s="27">
         <v>2012</v>
       </c>
-      <c r="L63" s="29">
+      <c r="L63" s="38">
         <f t="shared" si="14"/>
         <v>2.996262622279652</v>
       </c>
-      <c r="M63" s="36">
+      <c r="M63" s="33">
         <f t="shared" si="13"/>
         <v>1.1985397001162463</v>
       </c>
@@ -12010,14 +12019,14 @@
         <f t="shared" si="11"/>
         <v>5.5799047999999995E-3</v>
       </c>
-      <c r="K64" s="28">
+      <c r="K64" s="27">
         <v>2013</v>
       </c>
-      <c r="L64" s="29">
+      <c r="L64" s="38">
         <f t="shared" si="14"/>
         <v>4.6167868644626706</v>
       </c>
-      <c r="M64" s="36">
+      <c r="M64" s="33">
         <f t="shared" si="13"/>
         <v>1.8467681380424943</v>
       </c>
@@ -12052,14 +12061,14 @@
         <f t="shared" si="11"/>
         <v>5.604228450000001E-3</v>
       </c>
-      <c r="K65" s="28">
+      <c r="K65" s="27">
         <v>2014</v>
       </c>
-      <c r="L65" s="29">
+      <c r="L65" s="38">
         <f t="shared" si="14"/>
         <v>5.0528543574093927</v>
       </c>
-      <c r="M65" s="36">
+      <c r="M65" s="33">
         <f t="shared" si="13"/>
         <v>2.0212001782583693</v>
       </c>
@@ -12094,14 +12103,14 @@
         <f t="shared" si="11"/>
         <v>5.6572884500000007E-3</v>
       </c>
-      <c r="K66" s="28">
+      <c r="K66" s="27">
         <v>2015</v>
       </c>
-      <c r="L66" s="29">
+      <c r="L66" s="38">
         <f t="shared" si="14"/>
         <v>3.4527684650943073</v>
       </c>
-      <c r="M66" s="36">
+      <c r="M66" s="33">
         <f t="shared" si="13"/>
         <v>1.3811473166449033</v>
       </c>
@@ -12136,14 +12145,14 @@
         <f t="shared" si="11"/>
         <v>5.8319999999999995E-3</v>
       </c>
-      <c r="K67" s="28">
+      <c r="K67" s="27">
         <v>2016</v>
       </c>
-      <c r="L67" s="29">
+      <c r="L67" s="38">
         <f t="shared" si="14"/>
         <v>2.8118737454448515</v>
       </c>
-      <c r="M67" s="36">
+      <c r="M67" s="33">
         <f t="shared" si="13"/>
         <v>1.1247820169602178</v>
       </c>
@@ -12178,14 +12187,14 @@
         <f t="shared" si="11"/>
         <v>5.7212904499999995E-3</v>
       </c>
-      <c r="K68" s="28">
+      <c r="K68" s="27">
         <v>2017</v>
       </c>
-      <c r="L68" s="29">
+      <c r="L68" s="38">
         <f t="shared" si="14"/>
         <v>2.8886242909607867</v>
       </c>
-      <c r="M68" s="36">
+      <c r="M68" s="33">
         <f t="shared" si="13"/>
         <v>1.1554831227719773</v>
       </c>
@@ -12220,14 +12229,14 @@
         <f t="shared" ref="I69:I70" si="15">H69/2</f>
         <v>5.8007220500000001E-3</v>
       </c>
-      <c r="K69" s="28">
+      <c r="K69" s="27">
         <v>2018</v>
       </c>
-      <c r="L69" s="29">
+      <c r="L69" s="38">
         <f t="shared" si="14"/>
         <v>2.2108781653720939</v>
       </c>
-      <c r="M69" s="36">
+      <c r="M69" s="33">
         <f t="shared" si="13"/>
         <v>0.88437683453213278</v>
       </c>
@@ -12262,14 +12271,14 @@
         <f t="shared" si="15"/>
         <v>5.7266402000000008E-3</v>
       </c>
-      <c r="K70" s="28">
+      <c r="K70" s="27">
         <v>2019</v>
       </c>
-      <c r="L70" s="29">
+      <c r="L70" s="38">
         <f t="shared" si="14"/>
         <v>2.7412820560909119</v>
       </c>
-      <c r="M70" s="36">
+      <c r="M70" s="33">
         <f t="shared" si="13"/>
         <v>1.0965445248392507</v>
       </c>
@@ -12304,14 +12313,14 @@
         <f>H71/2</f>
         <v>5.6849784500000002E-3</v>
       </c>
-      <c r="K71" s="30">
+      <c r="K71" s="28">
         <v>2020</v>
       </c>
-      <c r="L71" s="31">
+      <c r="L71" s="37">
         <f t="shared" si="14"/>
         <v>3.1341689552540397</v>
       </c>
-      <c r="M71" s="37">
+      <c r="M71" s="34">
         <f t="shared" si="13"/>
         <v>1.2537038281663766</v>
       </c>
@@ -12394,7 +12403,7 @@
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A77" s="32" t="s">
+      <c r="A77" s="29" t="s">
         <v>29</v>
       </c>
     </row>
@@ -12427,10 +12436,10 @@
       </c>
       <c r="J80" s="24"/>
       <c r="K80" s="25"/>
-      <c r="L80" s="26" t="s">
+      <c r="L80" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="M80" s="27" t="s">
+      <c r="M80" s="26" t="s">
         <v>38</v>
       </c>
       <c r="N80" s="24"/>
@@ -12465,14 +12474,14 @@
         <f>H81/2</f>
         <v>1.3706712449999998E-2</v>
       </c>
-      <c r="K81" s="28">
+      <c r="K81" s="27">
         <v>2006</v>
       </c>
-      <c r="L81" s="29">
+      <c r="L81" s="38">
         <f>EXP(B81+I81)</f>
         <v>8.8908877011474111E-2</v>
       </c>
-      <c r="M81" s="36">
+      <c r="M81" s="33">
         <f>L81/AVERAGE($L$81:$L$95)</f>
         <v>0.31124411355755044</v>
       </c>
@@ -12507,14 +12516,14 @@
         <f t="shared" ref="I82:I95" si="17">H82/2</f>
         <v>2.0228649800000002E-2</v>
       </c>
-      <c r="K82" s="28">
+      <c r="K82" s="27">
         <v>2007</v>
       </c>
-      <c r="L82" s="29">
+      <c r="L82" s="38">
         <f>EXP($B$81+$I$81+B82+I82)</f>
         <v>0.14871781350770713</v>
       </c>
-      <c r="M82" s="36">
+      <c r="M82" s="33">
         <f t="shared" ref="M82:M95" si="18">L82/AVERAGE($L$81:$L$95)</f>
         <v>0.52061780095872512</v>
       </c>
@@ -12546,14 +12555,14 @@
         <f t="shared" si="17"/>
         <v>2.2052100049999999E-2</v>
       </c>
-      <c r="K83" s="28">
+      <c r="K83" s="27">
         <v>2008</v>
       </c>
-      <c r="L83" s="29">
+      <c r="L83" s="38">
         <f t="shared" ref="L83:L95" si="19">EXP($B$81+$I$81+B83+I83)</f>
         <v>0.11538035336948967</v>
       </c>
-      <c r="M83" s="36">
+      <c r="M83" s="33">
         <f t="shared" si="18"/>
         <v>0.40391305135716865</v>
       </c>
@@ -12588,14 +12597,14 @@
         <f t="shared" si="17"/>
         <v>1.5190245000000002E-2</v>
       </c>
-      <c r="K84" s="28">
+      <c r="K84" s="27">
         <v>2009</v>
       </c>
-      <c r="L84" s="29">
+      <c r="L84" s="38">
         <f t="shared" si="19"/>
         <v>0.14796891773919907</v>
       </c>
-      <c r="M84" s="36">
+      <c r="M84" s="33">
         <f t="shared" si="18"/>
         <v>0.51799613473763217</v>
       </c>
@@ -12627,14 +12636,14 @@
         <f t="shared" si="17"/>
         <v>1.6585668449999997E-2</v>
       </c>
-      <c r="K85" s="28">
+      <c r="K85" s="27">
         <v>2010</v>
       </c>
-      <c r="L85" s="29">
+      <c r="L85" s="38">
         <f t="shared" si="19"/>
         <v>9.8222730482353901E-2</v>
       </c>
-      <c r="M85" s="36">
+      <c r="M85" s="33">
         <f t="shared" si="18"/>
         <v>0.34384920502636718</v>
       </c>
@@ -12669,14 +12678,14 @@
         <f t="shared" si="17"/>
         <v>1.9284516050000002E-2</v>
       </c>
-      <c r="K86" s="28">
+      <c r="K86" s="27">
         <v>2011</v>
       </c>
-      <c r="L86" s="29">
+      <c r="L86" s="38">
         <f t="shared" si="19"/>
         <v>6.3317167916094208E-2</v>
       </c>
-      <c r="M86" s="36">
+      <c r="M86" s="33">
         <f t="shared" si="18"/>
         <v>0.22165498500758277</v>
       </c>
@@ -12711,14 +12720,14 @@
         <f t="shared" si="17"/>
         <v>1.4627340799999999E-2</v>
       </c>
-      <c r="K87" s="28">
+      <c r="K87" s="27">
         <v>2012</v>
       </c>
-      <c r="L87" s="29">
+      <c r="L87" s="38">
         <f t="shared" si="19"/>
         <v>0.85905189397037818</v>
       </c>
-      <c r="M87" s="36">
+      <c r="M87" s="33">
         <f t="shared" si="18"/>
         <v>3.0072907703495022</v>
       </c>
@@ -12753,14 +12762,14 @@
         <f t="shared" si="17"/>
         <v>1.6514713800000001E-2</v>
       </c>
-      <c r="K88" s="28">
+      <c r="K88" s="27">
         <v>2013</v>
       </c>
-      <c r="L88" s="29">
+      <c r="L88" s="38">
         <f t="shared" si="19"/>
         <v>0.33952130708882516</v>
       </c>
-      <c r="M88" s="36">
+      <c r="M88" s="33">
         <f t="shared" si="18"/>
         <v>1.1885653245302437</v>
       </c>
@@ -12792,14 +12801,14 @@
         <f t="shared" si="17"/>
         <v>2.1984948049999998E-2</v>
       </c>
-      <c r="K89" s="28">
+      <c r="K89" s="27">
         <v>2014</v>
       </c>
-      <c r="L89" s="29">
+      <c r="L89" s="38">
         <f t="shared" si="19"/>
         <v>0.12326382037323932</v>
       </c>
-      <c r="M89" s="36">
+      <c r="M89" s="33">
         <f t="shared" si="18"/>
         <v>0.4315107759243747</v>
       </c>
@@ -12834,14 +12843,14 @@
         <f t="shared" si="17"/>
         <v>1.7758585799999997E-2</v>
       </c>
-      <c r="K90" s="28">
+      <c r="K90" s="27">
         <v>2015</v>
       </c>
-      <c r="L90" s="29">
+      <c r="L90" s="38">
         <f t="shared" si="19"/>
         <v>0.22271224949803139</v>
       </c>
-      <c r="M90" s="36">
+      <c r="M90" s="33">
         <f t="shared" si="18"/>
         <v>0.77965079532471193</v>
       </c>
@@ -12876,14 +12885,14 @@
         <f t="shared" si="17"/>
         <v>1.6523802050000001E-2</v>
       </c>
-      <c r="K91" s="28">
+      <c r="K91" s="27">
         <v>2016</v>
       </c>
-      <c r="L91" s="29">
+      <c r="L91" s="38">
         <f t="shared" si="19"/>
         <v>0.35919513540677045</v>
       </c>
-      <c r="M91" s="36">
+      <c r="M91" s="33">
         <f t="shared" si="18"/>
         <v>1.2574376740742836</v>
       </c>
@@ -12918,14 +12927,14 @@
         <f t="shared" si="17"/>
         <v>1.6033032450000002E-2</v>
       </c>
-      <c r="K92" s="28">
+      <c r="K92" s="27">
         <v>2017</v>
       </c>
-      <c r="L92" s="29">
+      <c r="L92" s="38">
         <f t="shared" si="19"/>
         <v>0.3501546884630693</v>
       </c>
-      <c r="M92" s="36">
+      <c r="M92" s="33">
         <f t="shared" si="18"/>
         <v>1.2257896993192634</v>
       </c>
@@ -12960,14 +12969,14 @@
         <f t="shared" si="17"/>
         <v>1.8578208799999999E-2</v>
       </c>
-      <c r="K93" s="28">
+      <c r="K93" s="27">
         <v>2018</v>
       </c>
-      <c r="L93" s="29">
+      <c r="L93" s="38">
         <f t="shared" si="19"/>
         <v>0.17623004232267206</v>
       </c>
-      <c r="M93" s="36">
+      <c r="M93" s="33">
         <f t="shared" si="18"/>
         <v>0.61693011034039869</v>
       </c>
@@ -13002,14 +13011,14 @@
         <f t="shared" si="17"/>
         <v>1.511191125E-2</v>
       </c>
-      <c r="K94" s="28">
+      <c r="K94" s="27">
         <v>2019</v>
       </c>
-      <c r="L94" s="29">
+      <c r="L94" s="38">
         <f t="shared" si="19"/>
         <v>0.56511197801272917</v>
       </c>
-      <c r="M94" s="36">
+      <c r="M94" s="33">
         <f t="shared" si="18"/>
         <v>1.9782926358931141</v>
       </c>
@@ -13044,14 +13053,14 @@
         <f t="shared" si="17"/>
         <v>1.4936832799999999E-2</v>
       </c>
-      <c r="K95" s="30">
+      <c r="K95" s="28">
         <v>2020</v>
       </c>
-      <c r="L95" s="31">
+      <c r="L95" s="37">
         <f t="shared" si="19"/>
         <v>0.62708921816369867</v>
       </c>
-      <c r="M95" s="37">
+      <c r="M95" s="34">
         <f t="shared" si="18"/>
         <v>2.1952569235990813</v>
       </c>

</xml_diff>